<commit_message>
Ponpeco Accessories - 3298397484 업데이트
</commit_message>
<xml_diff>
--- a/Data/Ponpeco Accessories - 3298397484/3298397484.xlsx
+++ b/Data/Ponpeco Accessories - 3298397484/3298397484.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Pull Request Here\Ponpeco Accessories - 3298397484\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Ponpeco Accessories - 3298397484\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C861526-A5D4-4FDD-A6AC-A7A3C6B09838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F35650E-8731-4A07-A08C-53DA72AB722B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240925" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,96 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>bjmi0</author>
+  </authors>
+  <commentList>
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-14 이전의 원문: 'PAG EyepatchL'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-14 이전의 원문: 'A stylish eyepatch. It has a small hole, so it doesn't affect your vision. It offers minimal eye protection, so don't rely on it too much.'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-14 이전의 원문: 'PAG EyepatchR'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-14 이전의 원문: 'A stylish eyepatch. It has a small hole, so it doesn't affect your vision. It offers minimal eye protection, so don't rely on it too much.'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E55" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-14에 새로 추가된 노드들 (8개)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F55" authorId="0" shapeId="0" xr:uid="{606C03B8-9F65-42B5-B088-2B8602931183}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-14에 새로 추가된 노드들 (8개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="243">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -52,147 +140,147 @@
     <t>PAE Teardrop Earrings</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>물방울 귀걸이</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAETeardropEarrings.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>물방울 귀걸이</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAETeardropEarrings.description</t>
   </si>
   <si>
     <t>Teardrop-shaped earrings. They have no effect when equipped.\n (*Note: They appear as ear accessories but are equipped in the 'Neck' slot.)</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>물방울 모양의 귀걸이입니다. 아무런 효과도 없습니다.\n(주의: 외관상 귀 아래에 표시되지만 목 슬롯에 장착됩니다)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAERodEarrings.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>물방울 모양의 귀걸이입니다. 아무런 효과도 없습니다.\n(주의: 외관상 귀 아래에 표시되지만 목 슬롯에 장착됩니다)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAERodEarrings.label</t>
   </si>
   <si>
     <t>PAE Rod Earrings</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>봉 귀걸이</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAERodEarrings.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>봉 귀걸이</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAERodEarrings.description</t>
   </si>
   <si>
     <t>Rod-shaped earrings. They have no effect when equipped. \n(*Note: They appear as ear accessories but are equipped in the 'Neck' slot.)</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>막대기 모양의 귀걸이입니다. 아무런 효과도 없습니다.\n(주의: 외관상 귀 아래에 표시되지만 목 슬롯에 장착됩니다)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAESmallEarrings.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>막대기 모양의 귀걸이입니다. 아무런 효과도 없습니다.\n(주의: 외관상 귀 아래에 표시되지만 목 슬롯에 장착됩니다)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAESmallEarrings.label</t>
   </si>
   <si>
     <t>PAE Small Earrings</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>소형 귀걸이</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAESmallEarrings.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>소형 귀걸이</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAESmallEarrings.description</t>
   </si>
   <si>
     <t>Simple, small earrings. They have no effect when equipped. \n(*Note: They appear as ear accessories but are equipped in the 'Neck' slot.)</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>작은 귀걸이입니다. 아무런 효과도 없습니다.\n(주의: 외관상 귀 아래에 표시되지만 목 슬롯에 장착됩니다)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAGSunglassesA.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>작은 귀걸이입니다. 아무런 효과도 없습니다.\n(주의: 외관상 귀 아래에 표시되지만 목 슬롯에 장착됩니다)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAGSunglassesA.label</t>
   </si>
   <si>
     <t>PAG Orange Sunglasses</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>주황색 선글라스</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAGSunglassesA.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>주황색 선글라스</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAGSunglassesA.description</t>
   </si>
   <si>
@@ -211,21 +299,21 @@
     <t>PAG Sunglasses</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>선글라스</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAGSunglassesB.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>선글라스</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAGSunglassesB.description</t>
   </si>
   <si>
@@ -244,21 +332,21 @@
     <t>PAG Glasses</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>안경</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAGGlasses.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>안경</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAGGlasses.description</t>
   </si>
   <si>
@@ -274,31 +362,16 @@
     <t>Apparel_PAGEyepatchL.label</t>
   </si>
   <si>
-    <t>PAG EyepatchL</t>
+    <t>A stylish eyepatch. It has a small hole, so it doesn't affect your vision. It offers minimal eye protection, so don't rely on it too much.Displayed above the hair.</t>
   </si>
   <si>
     <t>ThingDef+Apparel_PAGEyepatchL.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>안대 (왼쪽)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAGEyepatchL.description</t>
   </si>
   <si>
-    <t>A stylish eyepatch. It has a small hole, so it doesn't affect your vision. It offers minimal eye protection, so don't rely on it too much.</t>
-  </si>
-  <si>
-    <t>멋진 장식용 안대입니다. 가운데 구멍이 뚫려 있어 시력에 영향을 주지 않습니다. 방어구로써 성능은 크게 기대하지 않는 것이 좋습니다.</t>
+    <t>ThingDef+Apparel_PAGEyepatchLU.label</t>
   </si>
   <si>
     <t>ThingDef+Apparel_PAGEyepatchR.label</t>
@@ -307,24 +380,12 @@
     <t>Apparel_PAGEyepatchR.label</t>
   </si>
   <si>
-    <t>PAG EyepatchR</t>
+    <t>Apparel_PAGEyepatchLU.label</t>
   </si>
   <si>
     <t>ThingDef+Apparel_PAGEyepatchR.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>안대 (오른쪽)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAGEyepatchR.description</t>
   </si>
   <si>
@@ -337,21 +398,21 @@
     <t>PAH Hair Scarf</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>스카프</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAHHeadScarf.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>스카프</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAHHeadScarf.description</t>
   </si>
   <si>
@@ -370,69 +431,81 @@
     <t>PAH Hair Scarf with Lace</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>레이스 스카프</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAHHeadScarfB.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>레이스 스카프</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAHHeadScarfB.description</t>
   </si>
   <si>
     <t>A lace-adorned decorative headscarf. It offers similar coverage to a hood.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>레이스가 달린 장식용 스카프입니다. 두건과 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAHHeadband.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>레이스가 달린 장식용 스카프입니다. 두건과 비슷한 성능을 지녔습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAHHeadband.label</t>
   </si>
   <si>
     <t>PAH Simple Headband</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>단순한 머리띠</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAHHeadband.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>단순한 머리띠</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAHHeadband.description</t>
   </si>
   <si>
     <t>일자로 뻗은 머리띠입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>A straightforward headband. It offers similar functionality to a tribal headdress.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAHRibbonHeadband.label</t>
   </si>
   <si>
@@ -442,21 +515,21 @@
     <t>PAH Ribbon Headband</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>리본 머리띠</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAHRibbonHeadband.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>리본 머리띠</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAHRibbonHeadband.description</t>
   </si>
   <si>
@@ -475,21 +548,21 @@
     <t>PAH Big Ribbon</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>큰 리본</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAHDekaRibbon.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>큰 리본</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAHDekaRibbon.description</t>
   </si>
   <si>
@@ -499,27 +572,39 @@
     <t>ThingDef+Apparel_PAHMokoRibbon.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>커다란 리본 모양 머리장식입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAHMokoRibbon.label</t>
   </si>
   <si>
     <t>PAH Fluffy Ribbon Headband</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>털 리본 머리띠</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAHMokoRibbon.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>털 리본 머리띠</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAHMokoRibbon.description</t>
   </si>
   <si>
@@ -529,321 +614,333 @@
     <t>ThingDef+Apparel_PAHHeadphones.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>푹신한 리본이 달린 머리띠입니다. 털모자와 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAHHeadphones.label</t>
   </si>
   <si>
     <t>PAH Headphones</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>헤드폰</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAHHeadphones.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>헤드폰</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAHHeadphones.description</t>
   </si>
   <si>
     <t>Fashionable headphones designed purely for style. They do not block surrounding sounds and provide protection similar to a simple helmet.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>순전히 장식용으로 만들어진 헤드폰입니다. 노이즈캔슬링 기능은 존재하지 않으며 간단한 헬멧 수준의 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAHVeil.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>순전히 장식용으로 만들어진 헤드폰입니다. 노이즈캔슬링 기능은 존재하지 않으며 간단한 헬멧 수준의 성능을 지녔습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAHVeil.label</t>
   </si>
   <si>
     <t>PAH Veil</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>베일</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAHVeil.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>베일</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAHVeil.description</t>
   </si>
   <si>
     <t>A mysterious lace-adorned veil. It offers similar coverage to a hood.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>신비한 분위기를 주는 베일입니다. 두건과 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAMHairExtensions.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>신비한 분위기를 주는 베일입니다. 두건과 비슷한 성능을 지녔습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAMHairExtensions.label</t>
   </si>
   <si>
     <t>PAM Hair Extensions</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>머리카락 장식</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAMHairExtensions.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>머리카락 장식</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAMHairExtensions.description</t>
   </si>
   <si>
     <t>Hair extensions that add an accent to your hairstyle. It has no effect when equipped.\n (*Note: Equipped in the 'Neck' slot.)</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>머리카락에 포인트를 주기 위해 사용합니다. 아무런 효과도 없습니다.\n (주의: 목 슬롯에 장착됩니다)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAMRibbonPin.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>머리카락에 포인트를 주기 위해 사용합니다. 아무런 효과도 없습니다.\n (주의: 목 슬롯에 장착됩니다)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAMRibbonPin.label</t>
   </si>
   <si>
     <t>PAM Ribbon Pin</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>리본 머리핀</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAMRibbonPin.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>리본 머리핀</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAMRibbonPin.description</t>
   </si>
   <si>
     <t>A hairpin shaped like a ribbon. It has no effect when equipped. \n(*Note: Equipped in the 'Neck' slot.)</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>리본 모양 머리핀입니다. 아무런 효과도 없습니다.\n(주의: 목 슬롯에 장착됩니다)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAMStarHairPin.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>리본 모양 머리핀입니다. 아무런 효과도 없습니다.\n(주의: 목 슬롯에 장착됩니다)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAMStarHairPin.label</t>
   </si>
   <si>
     <t>PAM Star Hair Pin</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>별 머리핀</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAMStarHairPin.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>별 머리핀</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAMStarHairPin.description</t>
   </si>
   <si>
     <t>A hairpin shaped like a star. It has no effect when equipped. \n(*Note: Equipped in the 'Neck' slot.)</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>별 모양 머리핀입니다. 아무런 효과도 없습니다.\n(주의: 목 슬롯에 장착됩니다)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAMCloverCrown.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>별 모양 머리핀입니다. 아무런 효과도 없습니다.\n(주의: 목 슬롯에 장착됩니다)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAMCloverCrown.label</t>
   </si>
   <si>
     <t>PAM Clover Crown</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>클로버 머리띠</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAMCloverCrown.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>클로버 머리띠</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PAMCloverCrown.description</t>
   </si>
   <si>
     <t>A flower crown made of white clover. It has no effect when equipped. \n(*Note: Equipped in the 'Neck' slot.)</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>하얀 클로버로 만든 머리띠입니다. 아무런 효과도 없습니다.\n(주의: 목 슬롯에 장착됩니다)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PANMuffler.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>하얀 클로버로 만든 머리띠입니다. 아무런 효과도 없습니다.\n(주의: 목 슬롯에 장착됩니다)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PANMuffler.label</t>
   </si>
   <si>
     <t>PAN Muffler</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>머플러</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PANMuffler.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>머플러</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PANMuffler.description</t>
   </si>
   <si>
     <t>This muffler offers a slight warming effect but provides little to no defense.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>몸을 약간이나마 따뜻하게 만들어 주는 머플러입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PANNeckScarf.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>몸을 약간이나마 따뜻하게 만들어 주는 머플러입니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PANNeckScarf.label</t>
   </si>
   <si>
     <t>PAN Neck Scarf</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>목 스카프</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PANNeckScarf.description</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>목 스카프</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Apparel_PANNeckScarf.description</t>
   </si>
   <si>
@@ -865,6 +962,18 @@
     <t>ThingDef+Apparel_PAHDeepHood.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>큰 두건</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAHDeepHood.description</t>
   </si>
   <si>
@@ -874,6 +983,18 @@
     <t>ThingDef+Apparel_PAHPilotGoggles.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>푹 눌러쓰면 얼굴을 가릴 수 있는 후드입니다. 수줍음이 많은 사람들을 위해 만들어졌습니다. 두건과 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAHPilotGoggles.label</t>
   </si>
   <si>
@@ -883,6 +1004,18 @@
     <t>ThingDef+Apparel_PAHPilotGoggles.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>조종사 고글</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAHPilotGoggles.description</t>
   </si>
   <si>
@@ -892,6 +1025,18 @@
     <t>ThingDef+Apparel_PAHHeaddress.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>특별한 이유로 눈이 아니라 이마 위에 걸치는 용도로 설계된 조종사 고글입니다. 놀랍게도 방탄모와 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAHHeaddress.label</t>
   </si>
   <si>
@@ -901,6 +1046,18 @@
     <t>ThingDef+Apparel_PAHHeaddress.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>헤드 드레스</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAHHeaddress.description</t>
   </si>
   <si>
@@ -910,6 +1067,18 @@
     <t>ThingDef+Apparel_PAHAngolaBeret.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>고딕 로리타 스타일의 리본과 레이스로 장식된 머리 장식입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAHAngolaBeret.label</t>
   </si>
   <si>
@@ -919,54 +1088,151 @@
     <t>ThingDef+Apparel_PAHAngolaBeret.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>앙골라 베레모</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAHAngolaBeret.description</t>
   </si>
   <si>
-    <t>푹 눌러쓰면 얼굴을 가릴 수 있는 후드입니다. 수줍음이 많은 사람들을 위해 만들어졌습니다. 두건과 비슷한 성능을 지녔습니다.</t>
+    <t>PAG EyepatchL Over</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>A fluffy and soft angora beret that provides warmth. It has the same stats as a tuque.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>푹신하고 따뜻한 베레모입니다. 털모자와 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>PAG EyepatchR Over</t>
+  </si>
+  <si>
+    <t>PAG EyepatchL Under</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAGEyepatchLU.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAGEyepatchLU.description</t>
+  </si>
+  <si>
+    <t>A stylish eyepatch. It has a small hole, so it doesn't affect your vision. It offers minimal eye protection, so don't rely on it too much. Displayed below the hair.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAGEyepatchRU.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAGEyepatchRU.label</t>
+  </si>
+  <si>
+    <t>PAG EyepatchR Under</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAGEyepatchRU.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAGEyepatchRU.description</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHTiara.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHTiara.label</t>
+  </si>
+  <si>
+    <t>PAH Tiara</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHTiara.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHTiara.description</t>
+  </si>
+  <si>
+    <t>A finely crafted metal tiara adorned with delicate details. Functions similarly to the Coronet.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMFloralPin.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAMFloralPin.label</t>
+  </si>
+  <si>
+    <t>PAM Floral Pin</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMFloralPin.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAMFloralPin.description</t>
+  </si>
+  <si>
+    <t>A delicate flower-shaped hairpiece that brings subtle charm to the face. Crafted from fabric and faux leather for lasting use. It has no effect when equipped. \n(*Note: Equipped in the 'Neck' slot.)</t>
+  </si>
+  <si>
+    <t>안대 (왼쪽 위)</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>안대 (오른쪽 위)</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>안대 (왼쪽 아래)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>큰 두건</t>
+    <t>안대 (오른쪽 아래)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>조종사 고글</t>
+    <t>멋진 장식용 안대입니다. 가운데 구멍이 뚫려 있어 시력에 영향을 주지 않습니다. 방어구로써 성능은 크게 기대하지 않는 것이 좋습니다. 머리카락 위에 표시됩니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>특별한 이유로 눈이 아니라 이마 위에 걸치는 용도로 설계된 조종사 고글입니다. 놀랍게도 방탄모와 비슷한 성능을 지녔습니다.</t>
+    <t>멋진 장식용 안대입니다. 가운데 구멍이 뚫려 있어 시력에 영향을 주지 않습니다. 방어구로써 성능은 크게 기대하지 않는 것이 좋습니다. 머리카락 아래에 표시됩니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>헤드 드레스</t>
+    <t>티아라</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>A straightforward headband. It offers similar functionality to a tribal headdress.</t>
+    <t>섬세한 장식으로 정교하게 제작된 금속 티아라입니다. 장식관과 성능이 비슷합니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>커다란 리본 모양 머리장식입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
+    <t>꽃핀</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>고딕 로리타 스타일의 리본과 레이스로 장식된 머리 장식입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>앙골라 베레모</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A fluffy and soft angora beret that provides warmth. It has the same stats as a tuque.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>푹신한 리본이 달린 머리띠입니다. 털모자와 비슷한 성능을 지녔습니다.</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>푹신하고 따뜻한 베레모입니다. 털모자와 비슷한 성능을 지녔습니다.</t>
+    <t>얼굴에 은은한 매력을 더하는 섬세한 꽃 모양 머리 장식입니다. 천과 인조 가죽으로 제작되어 오래도록 사용할 수 있습니다. 장착 시 아무런 효과도 없습니다. \n(*참고: '목' 슬롯에 장착됩니다.)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -974,7 +1240,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -993,8 +1259,14 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1004,6 +1276,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF87CEEB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
       </patternFill>
     </fill>
   </fills>
@@ -1019,10 +1296,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1324,11 +1602,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1339,7 +1617,8 @@
     <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.08984375" style="1" customWidth="1"/>
     <col min="6" max="6" width="46.54296875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -1376,12 +1655,12 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -1393,12 +1672,12 @@
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -1410,12 +1689,12 @@
         <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -1427,12 +1706,12 @@
         <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -1444,12 +1723,12 @@
         <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -1461,12 +1740,12 @@
         <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -1478,12 +1757,12 @@
         <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
@@ -1512,12 +1791,12 @@
         <v>41</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
@@ -1546,12 +1825,12 @@
         <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -1576,11 +1855,11 @@
       <c r="C14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>57</v>
+      <c r="E14" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>59</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -1591,234 +1870,234 @@
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>62</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>211</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>67</v>
+        <v>234</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>62</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="F22" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="E25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="E27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -1829,18 +2108,18 @@
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="F29" s="1" t="s">
-        <v>211</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>7</v>
@@ -1852,12 +2131,12 @@
         <v>116</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
@@ -1869,12 +2148,12 @@
         <v>120</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>7</v>
@@ -1886,12 +2165,12 @@
         <v>124</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>7</v>
@@ -1903,12 +2182,12 @@
         <v>128</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>7</v>
@@ -1920,12 +2199,12 @@
         <v>132</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>7</v>
@@ -1937,12 +2216,12 @@
         <v>136</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>7</v>
@@ -1954,12 +2233,12 @@
         <v>140</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>7</v>
@@ -1971,12 +2250,12 @@
         <v>144</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>7</v>
@@ -1988,12 +2267,12 @@
         <v>148</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>7</v>
@@ -2005,12 +2284,12 @@
         <v>152</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>7</v>
@@ -2022,12 +2301,12 @@
         <v>156</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>7</v>
@@ -2039,12 +2318,12 @@
         <v>160</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>7</v>
@@ -2056,12 +2335,12 @@
         <v>164</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>7</v>
@@ -2073,12 +2352,12 @@
         <v>168</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>7</v>
@@ -2090,12 +2369,12 @@
         <v>172</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>7</v>
@@ -2124,7 +2403,7 @@
         <v>180</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
@@ -2135,119 +2414,256 @@
         <v>7</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="F53" s="1" t="s">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A55" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>212</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A56" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A58" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A59" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A60" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A61" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A62" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ponpeco Accessories 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Ponpeco Accessories - 3298397484/3298397484.xlsx
+++ b/Data/Ponpeco Accessories - 3298397484/3298397484.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Ponpeco Accessories - 3298397484\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F35650E-8731-4A07-A08C-53DA72AB722B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1A8637-A9B0-45DD-8F48-B0709488DEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F55" authorId="0" shapeId="0" xr:uid="{606C03B8-9F65-42B5-B088-2B8602931183}">
+    <comment ref="F55" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -103,12 +103,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="E63" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-02에 새로 추가된 노드들 (22개)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F63" authorId="0" shapeId="0" xr:uid="{4550BFA6-FACB-4706-BBAB-F333630E2B79}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-02에 새로 추가된 노드들 (22개)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="331">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -362,783 +388,831 @@
     <t>Apparel_PAGEyepatchL.label</t>
   </si>
   <si>
+    <t>PAG EyepatchL Over</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAGEyepatchL.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>안대 (왼쪽 위)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PAGEyepatchL.description</t>
+  </si>
+  <si>
     <t>A stylish eyepatch. It has a small hole, so it doesn't affect your vision. It offers minimal eye protection, so don't rely on it too much.Displayed above the hair.</t>
   </si>
   <si>
-    <t>ThingDef+Apparel_PAGEyepatchL.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAGEyepatchL.description</t>
+    <t>ThingDef+Apparel_PAGEyepatchR.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>멋진 장식용 안대입니다. 가운데 구멍이 뚫려 있어 시력에 영향을 주지 않습니다. 방어구로써 성능은 크게 기대하지 않는 것이 좋습니다. 머리카락 위에 표시됩니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PAGEyepatchR.label</t>
+  </si>
+  <si>
+    <t>PAG EyepatchR Over</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAGEyepatchR.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>안대 (오른쪽 위)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PAGEyepatchR.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHHeadScarf.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHHeadScarf.label</t>
+  </si>
+  <si>
+    <t>PAH Hair Scarf</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>스카프</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHHeadScarf.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHHeadScarf.description</t>
+  </si>
+  <si>
+    <t>A stylish headscarf designed for decoration. It offers similar coverage to a hood.</t>
+  </si>
+  <si>
+    <t>장식용 스카프입니다. 두건과 비슷한 성능을 지녔습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHHeadScarfB.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHHeadScarfB.label</t>
+  </si>
+  <si>
+    <t>PAH Hair Scarf with Lace</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>레이스 스카프</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHHeadScarfB.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHHeadScarfB.description</t>
+  </si>
+  <si>
+    <t>A lace-adorned decorative headscarf. It offers similar coverage to a hood.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>레이스가 달린 장식용 스카프입니다. 두건과 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHHeadband.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHHeadband.label</t>
+  </si>
+  <si>
+    <t>PAH Simple Headband</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>단순한 머리띠</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHHeadband.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHHeadband.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>A straightforward headband. It offers similar functionality to a tribal headdress.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>일자로 뻗은 머리띠입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHRibbonHeadband.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHRibbonHeadband.label</t>
+  </si>
+  <si>
+    <t>PAH Ribbon Headband</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>리본 머리띠</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHRibbonHeadband.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHRibbonHeadband.description</t>
+  </si>
+  <si>
+    <t>It's a headband with a small ribbon. It offers similar functionality to a tribal headdress.</t>
+  </si>
+  <si>
+    <t>리본이 달린 머리띠입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHDekaRibbon.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHDekaRibbon.label</t>
+  </si>
+  <si>
+    <t>PAH Big Ribbon</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>큰 리본</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHDekaRibbon.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHDekaRibbon.description</t>
+  </si>
+  <si>
+    <t>A large ribbon-shaped hair ornament. It offers similar functionality to a tribal headdress.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>커다란 리본 모양 머리장식입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHMokoRibbon.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHMokoRibbon.label</t>
+  </si>
+  <si>
+    <t>PAH Fluffy Ribbon Headband</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>털 리본 머리띠</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHMokoRibbon.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHMokoRibbon.description</t>
+  </si>
+  <si>
+    <t>A headband with a fluffy ribbon. It functions similarly to a tuque.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>푹신한 리본이 달린 머리띠입니다. 털모자와 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHHeadphones.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHHeadphones.label</t>
+  </si>
+  <si>
+    <t>PAH Headphones</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>헤드폰</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHHeadphones.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHHeadphones.description</t>
+  </si>
+  <si>
+    <t>Fashionable headphones designed purely for style. They do not block surrounding sounds and provide protection similar to a simple helmet.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>순전히 장식용으로 만들어진 헤드폰입니다. 노이즈캔슬링 기능은 존재하지 않으며 간단한 헬멧 수준의 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHVeil.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHVeil.label</t>
+  </si>
+  <si>
+    <t>PAH Veil</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>베일</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHVeil.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHVeil.description</t>
+  </si>
+  <si>
+    <t>A mysterious lace-adorned veil. It offers similar coverage to a hood.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>신비한 분위기를 주는 베일입니다. 두건과 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMHairExtensions.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAMHairExtensions.label</t>
+  </si>
+  <si>
+    <t>PAM Hair Extensions</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>머리카락 장식</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMHairExtensions.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAMHairExtensions.description</t>
+  </si>
+  <si>
+    <t>Hair extensions that add an accent to your hairstyle. It has no effect when equipped.\n (*Note: Equipped in the 'Neck' slot.)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>머리카락에 포인트를 주기 위해 사용합니다. 아무런 효과도 없습니다.\n (주의: 목 슬롯에 장착됩니다)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMRibbonPin.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAMRibbonPin.label</t>
+  </si>
+  <si>
+    <t>PAM Ribbon Pin</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>리본 머리핀</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMRibbonPin.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAMRibbonPin.description</t>
+  </si>
+  <si>
+    <t>A hairpin shaped like a ribbon. It has no effect when equipped. \n(*Note: Equipped in the 'Neck' slot.)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>리본 모양 머리핀입니다. 아무런 효과도 없습니다.\n(주의: 목 슬롯에 장착됩니다)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMStarHairPin.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAMStarHairPin.label</t>
+  </si>
+  <si>
+    <t>PAM Star Hair Pin</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>별 머리핀</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMStarHairPin.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAMStarHairPin.description</t>
+  </si>
+  <si>
+    <t>A hairpin shaped like a star. It has no effect when equipped. \n(*Note: Equipped in the 'Neck' slot.)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>별 모양 머리핀입니다. 아무런 효과도 없습니다.\n(주의: 목 슬롯에 장착됩니다)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMCloverCrown.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAMCloverCrown.label</t>
+  </si>
+  <si>
+    <t>PAM Clover Crown</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>클로버 머리띠</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMCloverCrown.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAMCloverCrown.description</t>
+  </si>
+  <si>
+    <t>A flower crown made of white clover. It has no effect when equipped. \n(*Note: Equipped in the 'Neck' slot.)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>하얀 클로버로 만든 머리띠입니다. 아무런 효과도 없습니다.\n(주의: 목 슬롯에 장착됩니다)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PANMuffler.label</t>
+  </si>
+  <si>
+    <t>Apparel_PANMuffler.label</t>
+  </si>
+  <si>
+    <t>PAN Muffler</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>머플러</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PANMuffler.description</t>
+  </si>
+  <si>
+    <t>Apparel_PANMuffler.description</t>
+  </si>
+  <si>
+    <t>This muffler offers a slight warming effect but provides little to no defense.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>몸을 약간이나마 따뜻하게 만들어 주는 머플러입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PANNeckScarf.label</t>
+  </si>
+  <si>
+    <t>Apparel_PANNeckScarf.label</t>
+  </si>
+  <si>
+    <t>PAN Neck Scarf</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>목 스카프</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PANNeckScarf.description</t>
+  </si>
+  <si>
+    <t>Apparel_PANNeckScarf.description</t>
+  </si>
+  <si>
+    <t>This scarf adds a stylish touch to your neck. It offers a slight warming effect but provides no defense.</t>
+  </si>
+  <si>
+    <t>목을 감싸는 두건입니다. 방어구로써 성능은 크게 기대하지 않는 것이 좋습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHDeepHood.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHDeepHood.label</t>
+  </si>
+  <si>
+    <t>PAH Deep Hood</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>큰 두건</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHDeepHood.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHDeepHood.description</t>
+  </si>
+  <si>
+    <t>A hood that is worn deep enough to hide the face. The wearer might be shy. It has the same stats as a hood.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>푹 눌러쓰면 얼굴을 가릴 수 있는 후드입니다. 수줍음이 많은 사람들을 위해 만들어졌습니다. 두건과 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHPilotGoggles.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHPilotGoggles.label</t>
+  </si>
+  <si>
+    <t>PAH Pilot Goggles</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>조종사 고글</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHPilotGoggles.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHPilotGoggles.description</t>
+  </si>
+  <si>
+    <t>Fashionable pilot goggles worn on the forehead instead of over the eyes, possibly for a specific reason. They have the same stats as a simple helmet.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>특별한 이유로 눈이 아니라 이마 위에 걸치는 용도로 설계된 조종사 고글입니다. 놀랍게도 방탄모와 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHHeaddress.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHHeaddress.label</t>
+  </si>
+  <si>
+    <t>PAH Headdress</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>헤드 드레스</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHHeaddress.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHHeaddress.description</t>
+  </si>
+  <si>
+    <t>A headdress adorned with Gothic Lolita-style ribbons and lace. It has the same stats as a tribal headdress.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>고딕 로리타 스타일의 리본과 레이스로 장식된 머리 장식입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHAngolaBeret.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHAngolaBeret.label</t>
+  </si>
+  <si>
+    <t>PAH Angola Beret</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>앙골라 베레모</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHAngolaBeret.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHAngolaBeret.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>A fluffy and soft angora beret that provides warmth. It has the same stats as a tuque.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>푹신하고 따뜻한 베레모입니다. 털모자와 비슷한 성능을 지녔습니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>ThingDef+Apparel_PAGEyepatchLU.label</t>
   </si>
   <si>
-    <t>ThingDef+Apparel_PAGEyepatchR.label</t>
-  </si>
-  <si>
-    <t>Apparel_PAGEyepatchR.label</t>
-  </si>
-  <si>
     <t>Apparel_PAGEyepatchLU.label</t>
   </si>
   <si>
-    <t>ThingDef+Apparel_PAGEyepatchR.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAGEyepatchR.description</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHHeadScarf.label</t>
-  </si>
-  <si>
-    <t>Apparel_PAHHeadScarf.label</t>
-  </si>
-  <si>
-    <t>PAH Hair Scarf</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>스카프</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHHeadScarf.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAHHeadScarf.description</t>
-  </si>
-  <si>
-    <t>A stylish headscarf designed for decoration. It offers similar coverage to a hood.</t>
-  </si>
-  <si>
-    <t>장식용 스카프입니다. 두건과 비슷한 성능을 지녔습니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHHeadScarfB.label</t>
-  </si>
-  <si>
-    <t>Apparel_PAHHeadScarfB.label</t>
-  </si>
-  <si>
-    <t>PAH Hair Scarf with Lace</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>레이스 스카프</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHHeadScarfB.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAHHeadScarfB.description</t>
-  </si>
-  <si>
-    <t>A lace-adorned decorative headscarf. It offers similar coverage to a hood.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>레이스가 달린 장식용 스카프입니다. 두건과 비슷한 성능을 지녔습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHHeadband.label</t>
-  </si>
-  <si>
-    <t>Apparel_PAHHeadband.label</t>
-  </si>
-  <si>
-    <t>PAH Simple Headband</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>단순한 머리띠</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHHeadband.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAHHeadband.description</t>
-  </si>
-  <si>
-    <t>일자로 뻗은 머리띠입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>A straightforward headband. It offers similar functionality to a tribal headdress.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHRibbonHeadband.label</t>
-  </si>
-  <si>
-    <t>Apparel_PAHRibbonHeadband.label</t>
-  </si>
-  <si>
-    <t>PAH Ribbon Headband</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>리본 머리띠</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHRibbonHeadband.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAHRibbonHeadband.description</t>
-  </si>
-  <si>
-    <t>It's a headband with a small ribbon. It offers similar functionality to a tribal headdress.</t>
-  </si>
-  <si>
-    <t>리본이 달린 머리띠입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHDekaRibbon.label</t>
-  </si>
-  <si>
-    <t>Apparel_PAHDekaRibbon.label</t>
-  </si>
-  <si>
-    <t>PAH Big Ribbon</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>큰 리본</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHDekaRibbon.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAHDekaRibbon.description</t>
-  </si>
-  <si>
-    <t>A large ribbon-shaped hair ornament. It offers similar functionality to a tribal headdress.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHMokoRibbon.label</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>커다란 리본 모양 머리장식입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apparel_PAHMokoRibbon.label</t>
-  </si>
-  <si>
-    <t>PAH Fluffy Ribbon Headband</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>털 리본 머리띠</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHMokoRibbon.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAHMokoRibbon.description</t>
-  </si>
-  <si>
-    <t>A headband with a fluffy ribbon. It functions similarly to a tuque.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHHeadphones.label</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>푹신한 리본이 달린 머리띠입니다. 털모자와 비슷한 성능을 지녔습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apparel_PAHHeadphones.label</t>
-  </si>
-  <si>
-    <t>PAH Headphones</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>헤드폰</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHHeadphones.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAHHeadphones.description</t>
-  </si>
-  <si>
-    <t>Fashionable headphones designed purely for style. They do not block surrounding sounds and provide protection similar to a simple helmet.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>순전히 장식용으로 만들어진 헤드폰입니다. 노이즈캔슬링 기능은 존재하지 않으며 간단한 헬멧 수준의 성능을 지녔습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHVeil.label</t>
-  </si>
-  <si>
-    <t>Apparel_PAHVeil.label</t>
-  </si>
-  <si>
-    <t>PAH Veil</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>베일</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHVeil.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAHVeil.description</t>
-  </si>
-  <si>
-    <t>A mysterious lace-adorned veil. It offers similar coverage to a hood.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>신비한 분위기를 주는 베일입니다. 두건과 비슷한 성능을 지녔습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAMHairExtensions.label</t>
-  </si>
-  <si>
-    <t>Apparel_PAMHairExtensions.label</t>
-  </si>
-  <si>
-    <t>PAM Hair Extensions</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>머리카락 장식</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAMHairExtensions.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAMHairExtensions.description</t>
-  </si>
-  <si>
-    <t>Hair extensions that add an accent to your hairstyle. It has no effect when equipped.\n (*Note: Equipped in the 'Neck' slot.)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>머리카락에 포인트를 주기 위해 사용합니다. 아무런 효과도 없습니다.\n (주의: 목 슬롯에 장착됩니다)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAMRibbonPin.label</t>
-  </si>
-  <si>
-    <t>Apparel_PAMRibbonPin.label</t>
-  </si>
-  <si>
-    <t>PAM Ribbon Pin</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>리본 머리핀</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAMRibbonPin.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAMRibbonPin.description</t>
-  </si>
-  <si>
-    <t>A hairpin shaped like a ribbon. It has no effect when equipped. \n(*Note: Equipped in the 'Neck' slot.)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>리본 모양 머리핀입니다. 아무런 효과도 없습니다.\n(주의: 목 슬롯에 장착됩니다)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAMStarHairPin.label</t>
-  </si>
-  <si>
-    <t>Apparel_PAMStarHairPin.label</t>
-  </si>
-  <si>
-    <t>PAM Star Hair Pin</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>별 머리핀</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAMStarHairPin.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAMStarHairPin.description</t>
-  </si>
-  <si>
-    <t>A hairpin shaped like a star. It has no effect when equipped. \n(*Note: Equipped in the 'Neck' slot.)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>별 모양 머리핀입니다. 아무런 효과도 없습니다.\n(주의: 목 슬롯에 장착됩니다)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAMCloverCrown.label</t>
-  </si>
-  <si>
-    <t>Apparel_PAMCloverCrown.label</t>
-  </si>
-  <si>
-    <t>PAM Clover Crown</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>클로버 머리띠</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAMCloverCrown.description</t>
-  </si>
-  <si>
-    <t>Apparel_PAMCloverCrown.description</t>
-  </si>
-  <si>
-    <t>A flower crown made of white clover. It has no effect when equipped. \n(*Note: Equipped in the 'Neck' slot.)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>하얀 클로버로 만든 머리띠입니다. 아무런 효과도 없습니다.\n(주의: 목 슬롯에 장착됩니다)</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PANMuffler.label</t>
-  </si>
-  <si>
-    <t>Apparel_PANMuffler.label</t>
-  </si>
-  <si>
-    <t>PAN Muffler</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>머플러</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PANMuffler.description</t>
-  </si>
-  <si>
-    <t>Apparel_PANMuffler.description</t>
-  </si>
-  <si>
-    <t>This muffler offers a slight warming effect but provides little to no defense.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>몸을 약간이나마 따뜻하게 만들어 주는 머플러입니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PANNeckScarf.label</t>
-  </si>
-  <si>
-    <t>Apparel_PANNeckScarf.label</t>
-  </si>
-  <si>
-    <t>PAN Neck Scarf</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>목 스카프</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PANNeckScarf.description</t>
-  </si>
-  <si>
-    <t>Apparel_PANNeckScarf.description</t>
-  </si>
-  <si>
-    <t>This scarf adds a stylish touch to your neck. It offers a slight warming effect but provides no defense.</t>
-  </si>
-  <si>
-    <t>목을 감싸는 두건입니다. 방어구로써 성능은 크게 기대하지 않는 것이 좋습니다.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHDeepHood.label</t>
-  </si>
-  <si>
-    <t>Apparel_PAHDeepHood.label</t>
-  </si>
-  <si>
-    <t>PAH Deep Hood</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHDeepHood.description</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>큰 두건</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apparel_PAHDeepHood.description</t>
-  </si>
-  <si>
-    <t>A hood that is worn deep enough to hide the face. The wearer might be shy. It has the same stats as a hood.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHPilotGoggles.label</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>푹 눌러쓰면 얼굴을 가릴 수 있는 후드입니다. 수줍음이 많은 사람들을 위해 만들어졌습니다. 두건과 비슷한 성능을 지녔습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apparel_PAHPilotGoggles.label</t>
-  </si>
-  <si>
-    <t>PAH Pilot Goggles</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHPilotGoggles.description</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>조종사 고글</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apparel_PAHPilotGoggles.description</t>
-  </si>
-  <si>
-    <t>Fashionable pilot goggles worn on the forehead instead of over the eyes, possibly for a specific reason. They have the same stats as a simple helmet.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHHeaddress.label</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>특별한 이유로 눈이 아니라 이마 위에 걸치는 용도로 설계된 조종사 고글입니다. 놀랍게도 방탄모와 비슷한 성능을 지녔습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apparel_PAHHeaddress.label</t>
-  </si>
-  <si>
-    <t>PAH Headdress</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHHeaddress.description</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>헤드 드레스</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apparel_PAHHeaddress.description</t>
-  </si>
-  <si>
-    <t>A headdress adorned with Gothic Lolita-style ribbons and lace. It has the same stats as a tribal headdress.</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHAngolaBeret.label</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>고딕 로리타 스타일의 리본과 레이스로 장식된 머리 장식입니다. 부족민의 머리 방어구와 비슷한 성능을 지녔습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apparel_PAHAngolaBeret.label</t>
-  </si>
-  <si>
-    <t>PAH Angola Beret</t>
-  </si>
-  <si>
-    <t>ThingDef+Apparel_PAHAngolaBeret.description</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>앙골라 베레모</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>Apparel_PAHAngolaBeret.description</t>
-  </si>
-  <si>
-    <t>PAG EyepatchL Over</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>A fluffy and soft angora beret that provides warmth. It has the same stats as a tuque.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>푹신하고 따뜻한 베레모입니다. 털모자와 비슷한 성능을 지녔습니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>PAG EyepatchR Over</t>
-  </si>
-  <si>
     <t>PAG EyepatchL Under</t>
   </si>
   <si>
     <t>ThingDef+Apparel_PAGEyepatchLU.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>안대 (왼쪽 아래)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAGEyepatchLU.description</t>
   </si>
   <si>
@@ -1148,6 +1222,18 @@
     <t>ThingDef+Apparel_PAGEyepatchRU.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>멋진 장식용 안대입니다. 가운데 구멍이 뚫려 있어 시력에 영향을 주지 않습니다. 방어구로써 성능은 크게 기대하지 않는 것이 좋습니다. 머리카락 아래에 표시됩니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAGEyepatchRU.label</t>
   </si>
   <si>
@@ -1157,21 +1243,45 @@
     <t>ThingDef+Apparel_PAGEyepatchRU.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>안대 (오른쪽 아래)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAGEyepatchRU.description</t>
   </si>
   <si>
+    <t>Apparel_PAHTiara.label</t>
+  </si>
+  <si>
     <t>ThingDef+Apparel_PAHTiara.label</t>
   </si>
   <si>
-    <t>Apparel_PAHTiara.label</t>
-  </si>
-  <si>
     <t>PAH Tiara</t>
   </si>
   <si>
     <t>ThingDef+Apparel_PAHTiara.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>티아라</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAHTiara.description</t>
   </si>
   <si>
@@ -1181,6 +1291,18 @@
     <t>ThingDef+Apparel_PAMFloralPin.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>섬세한 장식으로 정교하게 제작된 금속 티아라입니다. 장식관과 성능이 비슷합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAMFloralPin.label</t>
   </si>
   <si>
@@ -1190,49 +1312,317 @@
     <t>ThingDef+Apparel_PAMFloralPin.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>꽃핀</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Apparel_PAMFloralPin.description</t>
   </si>
   <si>
     <t>A delicate flower-shaped hairpiece that brings subtle charm to the face. Crafted from fabric and faux leather for lasting use. It has no effect when equipped. \n(*Note: Equipped in the 'Neck' slot.)</t>
   </si>
   <si>
-    <t>안대 (왼쪽 위)</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>안대 (오른쪽 위)</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>안대 (왼쪽 아래)</t>
+    <t>ThingDef+Apparel_PAHKnitHeadband.label</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>얼굴에 은은한 매력을 더하는 섬세한 꽃 모양 머리 장식입니다. 천과 인조 가죽으로 제작되어 오래도록 사용할 수 있습니다. 장착 시 아무런 효과도 없습니다. \n(*참고: '목' 슬롯에 장착됩니다.)</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Apparel_PAHKnitHeadband.label</t>
+  </si>
+  <si>
+    <t>PAH Knit Headband</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHKnitHeadband.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHKnitHeadband.description</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHPillboxHat.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHPillboxHat.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHPillboxHat.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHPillboxHat.description</t>
+  </si>
+  <si>
+    <t>A formal, brimless hat with a cylindrical shape.The delicate veil draped over the face adds an air of mystery.\nProvides the same stats as the Bowler Hat.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHFedora.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHFedora.label</t>
+  </si>
+  <si>
+    <t>PAH Fedora</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHFedora.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHFedora.description</t>
+  </si>
+  <si>
+    <t>A classic fedora, an essential part of a dashing gentleman's wardrobe.Perhaps it's also the first step toward becoming a detective or an adventurer.\nProvides the same stats as the Bowler Hat.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHFlatCap.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHFlatCap.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHFlatCap.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHFlatCap.description</t>
+  </si>
+  <si>
+    <t>A snug-fitting cap originally designed for hunting.\nIts flat top ensures it stays in place even during active movement.\nProvides the same stats as the Bowler Hat.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHCatEarNewsboy.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHCatEarNewsboy.label</t>
+  </si>
+  <si>
+    <t>PAH Cat Ear Newsboy</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHCatEarNewsboy.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHCatEarNewsboy.description</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHSailorBeret.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHSailorBeret.label</t>
+  </si>
+  <si>
+    <t>PAH Sailor Beret</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHSailorBeret.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHSailorBeret.description</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHMechaBunnyEars.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHMechaBunnyEars.label</t>
+  </si>
+  <si>
+    <t>PAH Mecha Bunny Ears</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHMechaBunnyEars.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHMechaBunnyEars.description</t>
+  </si>
+  <si>
+    <t>A high-tech headgear modeled after rabbit ears.\nEquipped with an electronically controlled fitting mechanism, it offers full head protection while remaining lightweight.\nFunctions the same as a Recon Helmet.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHHalfKitsuneMask.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAHHalfKitsuneMask.label</t>
+  </si>
+  <si>
+    <t>PAH Half Kitsune Mask</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAHHalfKitsuneMask.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAHHalfKitsuneMask.description</t>
+  </si>
+  <si>
+    <t>A fox-shaped mask reminiscent of those once used in the region known as “Japan” on old Earth.\nSomehow, its cultural legacy seems to live on even in this RimWorld.\nFunctions the same as a Mask.</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMRoseCrown.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAMRoseCrown.label</t>
+  </si>
+  <si>
+    <t>PAM Rose Crown</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMRoseCrown.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAMRoseCrown.description</t>
+  </si>
+  <si>
+    <t>An artificial crown shaped like blooming roses.\nIts unfading beauty gracefully adorns the wearer’s head.\nPurely decorative, with no functional effects.\n(*Note: Equipped in the 'Neck' slot.)</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMPartyHat.label</t>
+  </si>
+  <si>
+    <t>Apparel_PAMPartyHat.label</t>
+  </si>
+  <si>
+    <t>PAM Party Hat</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PAMPartyHat.description</t>
+  </si>
+  <si>
+    <t>Apparel_PAMPartyHat.description</t>
+  </si>
+  <si>
+    <t>A festive cone-shaped hat that sets the mood for celebration.\nWhy not wear it and party until the break of dawn?\nPurely decorative, with no functional effects. \n(*Note: Equipped in the 'Neck' slot.)</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PANFluffyMuffler.label</t>
+  </si>
+  <si>
+    <t>Apparel_PANFluffyMuffler.label</t>
+  </si>
+  <si>
+    <t>PAN Fluffy Muffler</t>
+  </si>
+  <si>
+    <t>ThingDef+Apparel_PANFluffyMuffler.description</t>
+  </si>
+  <si>
+    <t>Apparel_PANFluffyMuffler.description</t>
+  </si>
+  <si>
+    <t>A fluffy muffler with a soft and cozy texture.\nIts gentle material wraps warmly around the neck, offering a touch of comfort.\nProvides slight insulation, but offers no real protection.</t>
+  </si>
+  <si>
+    <t>A rib-knit headband.\nIt keeps stray bangs from falling into your face and breaking your focus, though it might just be a fashion statement.\nIt shares the same stats as a Tuque.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>안대 (오른쪽 아래)</t>
+    <t>두 개의 줄무늬와 리본이 특징인 선원 스타일 베레모입니다.\n중산모와 동일한 기능을 합니다.</t>
+  </si>
+  <si>
+    <t>활짝 핀 장미 모양의 인조 왕관입니다.\n시들지 않는 아름다움이 착용자의 머리를 우아하게 장식합니다.\n순전히 장식용이며, 기능적 효과는 없습니다.\n(*참고: '목' 부위에 장착됩니다.)</t>
+  </si>
+  <si>
+    <t>파티 모자</t>
+  </si>
+  <si>
+    <t>축제 분위기를 돋우는 원뿔 모양의 파티 모자입니다.\n이걸 쓰고 동틀 때까지 파티를 즐겨보는 건 어때요?\n순전히 장식용이며, 기능적 효과는 없습니다. \n(*참고: '목' 부위에 장착됩니다.)</t>
+  </si>
+  <si>
+    <t>복슬복슬 머플러</t>
+  </si>
+  <si>
+    <t>부드럽고 포근한 질감의 복슬복슬한 머플러입니다.\n부드러운 소재가 목을 따뜻하게 감싸 약간의 편안함을 제공합니다.\n약간의 단열 효과는 있지만, 실질적인 보호 기능은 없습니다.</t>
+  </si>
+  <si>
+    <t>A sailor-style beret featuring two stripes and a ribbon.\nFunctions the same as a Bowler Hat.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>멋진 장식용 안대입니다. 가운데 구멍이 뚫려 있어 시력에 영향을 주지 않습니다. 방어구로써 성능은 크게 기대하지 않는 것이 좋습니다. 머리카락 위에 표시됩니다.</t>
+    <t>니트 머리띠</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>멋진 장식용 안대입니다. 가운데 구멍이 뚫려 있어 시력에 영향을 주지 않습니다. 방어구로써 성능은 크게 기대하지 않는 것이 좋습니다. 머리카락 아래에 표시됩니다.</t>
+    <t>니트 재질의 머리띠입니다.\n흘러내리는 앞머리가 얼굴을 가려 집중을 방해하는 것을 막아줍니다. 물론 그냥 패션 아이템일 수도 있고요.\n털모자와 동일한 성능을 가집니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>티아라</t>
+    <t>PAH Pillbox Hat</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>섬세한 장식으로 정교하게 제작된 금속 티아라입니다. 장식관과 성능이 비슷합니다.</t>
+    <t>필박스 모자</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>꽃핀</t>
+    <t>원통형 모양의 챙 없는 정장 모자입니다.\n얼굴 위로 드리워진 섬세한 베일이 신비로운 분위기를 더합니다.\n중산모와 동일한 성능을 가집니다.</t>
+  </si>
+  <si>
+    <t>PAH Flat Cap</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>얼굴에 은은한 매력을 더하는 섬세한 꽃 모양 머리 장식입니다. 천과 인조 가죽으로 제작되어 오래도록 사용할 수 있습니다. 장착 시 아무런 효과도 없습니다. \n(*참고: '목' 슬롯에 장착됩니다.)</t>
+    <t>빵모자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A unique newsboy cap adorned with cat ears and decorative buttons.\nIts playful design adds a fun accent to any outfit.\nFunctions the same as a Bowler Hat.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>고양이 팔각모</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>고양이 귀와 장식용 단추로 꾸며진 독특한 팔각모입니다.\n장난기 넘치는 디자인이 어떤 옷차림에도 재미있는 포인트를 더해줍니다.\n중산모와 동일한 성능을 가집니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>중절모</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>클래식한 중절모로, 멋진 신사의 옷장에 필수적인 아이템입니다.\n어쩌면 탐정이나 모험가가 되기 위한 첫걸음일 수도 있겠네요.\n중산모와 동일한 성능을 가집니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>원래 사냥용으로 디자인된 모자입니다.\n평평한 윗부분 덕분에 활동적인 움직임 중에도 제자리에 고정됩니다.\n중산모와 동일한 성능을 가집니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>기계 토끼귀</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>토끼 귀를 본뜬 첨단 기술의 머리 장비입니다.\n전자 제어식 착용 메커니즘을 갖추고 있어, 가벼우면서도 머리 전체를 보호합니다.\n정찰대 헬멧과 동일한 기능을 합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>해양 베레모</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>과거 지구의 '일본'이라 불리던 지역에서 사용되었던 것을 연상시키는 여우 모양 가면입니다.\n어째서인지 그 문화적 유산은 이 림월드에서도 이어지는 것 같습니다.\n가면과 동일한 기능을 합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>여우 가면</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>장미 왕관</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1603,10 +1993,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1856,10 +2246,10 @@
         <v>56</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>208</v>
+        <v>57</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>233</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -1870,795 +2260,1169 @@
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>237</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>211</v>
+        <v>65</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>234</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>237</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>60</v>
+        <v>213</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>63</v>
+        <v>214</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>215</v>
-      </c>
       <c r="F58" s="1" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="F62" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
         <v>242</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A81" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A82" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A83" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A84" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>